<commit_message>
punish no stock ump more
</commit_message>
<xml_diff>
--- a/changes/ump.xlsx
+++ b/changes/ump.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACF3BCB-F61B-4972-96BD-ADDBBD5B7C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DB4F52-7871-41FD-B9FA-894FD2DB493C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>old</t>
   </si>
@@ -146,12 +146,6 @@
     <t>GHW Tailhook MOD 1</t>
   </si>
   <si>
-    <t>magpul_moe_carbine_stock</t>
-  </si>
-  <si>
-    <t>Magpul MOE Carbine</t>
-  </si>
-  <si>
     <t>ump45_std_200mm_barrel</t>
   </si>
   <si>
@@ -216,6 +210,9 @@
   </si>
   <si>
     <t>SilencerCo Omega45K</t>
+  </si>
+  <si>
+    <t>MOE Carbine</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1056,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,20 +1183,20 @@
         <v>11</v>
       </c>
       <c r="Q3">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="R3">
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="S3">
-        <v>-9</v>
+        <v>-13</v>
       </c>
       <c r="Z3">
         <v>0</v>
       </c>
       <c r="AA3">
         <f t="shared" ref="AA3:AA25" si="1">P3-Q3*20-R3*0.8-S3*0.6-U3*5+V3*5+W3/300</f>
-        <v>16.399999999999999</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -1229,23 +1226,23 @@
         <v>17.600000000000001</v>
       </c>
       <c r="P4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q4">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="R4">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="S4">
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="Z4">
         <v>600</v>
       </c>
       <c r="AA4">
         <f t="shared" si="1"/>
-        <v>17.600000000000001</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -1285,69 +1282,100 @@
         <v>-19.399999999999999</v>
       </c>
       <c r="P6">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="Q6">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="R6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Z6">
         <v>1000</v>
       </c>
       <c r="AA6">
         <f t="shared" si="1"/>
-        <v>-12.6</v>
+        <v>-7.3999999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>17</v>
       </c>
       <c r="D7">
-        <v>0.19</v>
+        <v>0.36</v>
       </c>
       <c r="E7">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="F7">
-        <v>-8</v>
+        <v>-10</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
-        <v>25.2</v>
+        <v>24.6</v>
       </c>
       <c r="P7">
         <v>17</v>
       </c>
       <c r="Q7">
-        <v>0.19</v>
+        <v>0.36</v>
       </c>
       <c r="R7">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="S7">
-        <v>-8</v>
+        <v>-10</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
       </c>
       <c r="Z7">
-        <v>800</v>
+        <v>1400</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="1"/>
-        <v>25.2</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -1390,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1403,7 +1431,7 @@
       </c>
       <c r="AA9">
         <f t="shared" si="1"/>
-        <v>-3</v>
+        <v>-2.6</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
@@ -1433,7 +1461,7 @@
         <v>16.2</v>
       </c>
       <c r="P10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q10">
         <v>0.09</v>
@@ -1446,7 +1474,7 @@
       </c>
       <c r="AA10">
         <f t="shared" si="1"/>
-        <v>16.2</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
@@ -1461,10 +1489,10 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1525,10 +1553,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -1592,10 +1620,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>-4</v>
@@ -1666,10 +1694,10 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1730,10 +1758,10 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -1794,10 +1822,10 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>-4</v>
@@ -1868,10 +1896,10 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>5</v>
@@ -1924,10 +1952,10 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -1988,10 +2016,10 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23">
         <v>-2</v>
@@ -2052,10 +2080,10 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>-8</v>
@@ -2116,10 +2144,10 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>-8</v>

</xml_diff>